<commit_message>
remove index column in data
</commit_message>
<xml_diff>
--- a/data/scaled_staff_req.xlsx
+++ b/data/scaled_staff_req.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Winston/Desktop/schedule-finder/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732C144D-5667-5840-8EF5-FDB11310C0F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="8920" yWindow="1660" windowWidth="32500" windowHeight="18640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -67,11 +73,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +143,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -183,7 +197,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -215,9 +229,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -249,6 +281,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -424,120 +474,122 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AB11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2">
+        <v>44204</v>
+      </c>
       <c r="H1" s="2">
-        <v>44204</v>
+        <v>44205</v>
       </c>
       <c r="I1" s="2">
-        <v>44205</v>
+        <v>44211</v>
       </c>
       <c r="J1" s="2">
-        <v>44211</v>
+        <v>44212</v>
       </c>
       <c r="K1" s="2">
-        <v>44212</v>
+        <v>44218</v>
       </c>
       <c r="L1" s="2">
-        <v>44218</v>
+        <v>44219</v>
       </c>
       <c r="M1" s="2">
-        <v>44219</v>
+        <v>44225</v>
       </c>
       <c r="N1" s="2">
-        <v>44225</v>
+        <v>44226</v>
       </c>
       <c r="O1" s="2">
-        <v>44226</v>
+        <v>44232</v>
       </c>
       <c r="P1" s="2">
-        <v>44232</v>
+        <v>44233</v>
       </c>
       <c r="Q1" s="2">
-        <v>44233</v>
+        <v>44239</v>
       </c>
       <c r="R1" s="2">
-        <v>44239</v>
+        <v>44240</v>
       </c>
       <c r="S1" s="2">
-        <v>44240</v>
+        <v>44246</v>
       </c>
       <c r="T1" s="2">
-        <v>44246</v>
+        <v>44247</v>
       </c>
       <c r="U1" s="2">
-        <v>44247</v>
+        <v>44253</v>
       </c>
       <c r="V1" s="2">
-        <v>44253</v>
+        <v>44254</v>
       </c>
       <c r="W1" s="2">
-        <v>43888</v>
+        <v>44260</v>
       </c>
       <c r="X1" s="2">
-        <v>44260</v>
+        <v>44261</v>
       </c>
       <c r="Y1" s="2">
-        <v>44261</v>
+        <v>44267</v>
       </c>
       <c r="Z1" s="2">
-        <v>44267</v>
+        <v>44268</v>
       </c>
       <c r="AA1" s="2">
-        <v>44268</v>
+        <v>44214</v>
       </c>
       <c r="AB1" s="2">
-        <v>44214</v>
-      </c>
-      <c r="AC1" s="2">
         <v>44242</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="H2">
         <v>-1</v>
@@ -549,37 +601,37 @@
         <v>-1</v>
       </c>
       <c r="K2">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="L2">
         <v>2</v>
       </c>
       <c r="M2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N2">
         <v>1</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P2">
         <v>2</v>
       </c>
       <c r="Q2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R2">
         <v>0</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T2">
         <v>2</v>
       </c>
       <c r="U2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V2">
         <v>1</v>
@@ -597,36 +649,33 @@
         <v>1</v>
       </c>
       <c r="AA2">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB2">
-        <v>-1</v>
-      </c>
-      <c r="AC2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -680,54 +729,51 @@
         <v>1</v>
       </c>
       <c r="Y3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Z3">
         <v>-1</v>
       </c>
       <c r="AA3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AB3">
         <v>1</v>
       </c>
-      <c r="AC3">
-        <v>1</v>
-      </c>
     </row>
-    <row r="4" spans="1:29">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J4">
         <v>-1</v>
       </c>
       <c r="K4">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -745,13 +791,13 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="R4">
         <v>-1</v>
       </c>
       <c r="S4">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -780,28 +826,25 @@
       <c r="AB4">
         <v>0</v>
       </c>
-      <c r="AC4">
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:29">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F5">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -810,13 +853,13 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5">
         <v>1</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -828,7 +871,7 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5">
         <v>1</v>
@@ -837,16 +880,16 @@
         <v>1</v>
       </c>
       <c r="R5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T5">
         <v>2</v>
       </c>
       <c r="U5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V5">
         <v>1</v>
@@ -864,54 +907,51 @@
         <v>1</v>
       </c>
       <c r="AA5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB5">
         <v>0</v>
       </c>
-      <c r="AC5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:29">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="F6">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L6">
         <v>2</v>
       </c>
       <c r="M6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N6">
         <v>1</v>
@@ -926,10 +966,10 @@
         <v>1</v>
       </c>
       <c r="R6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T6">
         <v>1</v>
@@ -956,19 +996,16 @@
         <v>1</v>
       </c>
       <c r="AB6">
-        <v>1</v>
-      </c>
-      <c r="AC6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
       <c r="C7">
         <v>2</v>
       </c>
@@ -976,13 +1013,13 @@
         <v>2</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H7">
         <v>-1</v>
@@ -994,31 +1031,31 @@
         <v>-1</v>
       </c>
       <c r="K7">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="L7">
         <v>1</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N7">
         <v>2</v>
       </c>
       <c r="O7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P7">
         <v>1</v>
       </c>
       <c r="Q7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7">
         <v>0</v>
       </c>
       <c r="S7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T7">
         <v>1</v>
@@ -1030,48 +1067,45 @@
         <v>1</v>
       </c>
       <c r="W7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X7">
         <v>2</v>
       </c>
       <c r="Y7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z7">
         <v>1</v>
       </c>
       <c r="AA7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB7">
-        <v>2</v>
-      </c>
-      <c r="AC7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
       <c r="C8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="E8">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -1086,7 +1120,7 @@
         <v>2</v>
       </c>
       <c r="L8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -1101,7 +1135,7 @@
         <v>1</v>
       </c>
       <c r="Q8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R8">
         <v>0</v>
@@ -1116,7 +1150,7 @@
         <v>0</v>
       </c>
       <c r="V8">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="W8">
         <v>-1</v>
@@ -1131,42 +1165,39 @@
         <v>-1</v>
       </c>
       <c r="AA8">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AB8">
         <v>1</v>
       </c>
-      <c r="AC8">
-        <v>1</v>
-      </c>
     </row>
-    <row r="9" spans="1:29">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
+      <c r="B9">
+        <v>-1</v>
+      </c>
       <c r="C9">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H9">
         <v>2</v>
       </c>
       <c r="I9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -1190,7 +1221,7 @@
         <v>1</v>
       </c>
       <c r="Q9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R9">
         <v>0</v>
@@ -1220,33 +1251,30 @@
         <v>0</v>
       </c>
       <c r="AA9">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB9">
         <v>-1</v>
       </c>
-      <c r="AC9">
-        <v>-1</v>
-      </c>
     </row>
-    <row r="10" spans="1:29">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -1255,19 +1283,19 @@
         <v>1</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J10">
         <v>2</v>
       </c>
       <c r="K10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L10">
         <v>1</v>
       </c>
       <c r="M10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -1279,7 +1307,7 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10">
         <v>1</v>
@@ -1303,33 +1331,30 @@
         <v>1</v>
       </c>
       <c r="Y10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z10">
         <v>0</v>
       </c>
       <c r="AA10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB10">
         <v>1</v>
       </c>
-      <c r="AC10">
-        <v>1</v>
-      </c>
     </row>
-    <row r="11" spans="1:29">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
       <c r="C11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -1338,25 +1363,25 @@
         <v>1</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J11">
         <v>-1</v>
       </c>
       <c r="K11">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="L11">
         <v>2</v>
       </c>
       <c r="M11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -1371,10 +1396,10 @@
         <v>1</v>
       </c>
       <c r="R11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11">
         <v>1</v>
@@ -1392,18 +1417,15 @@
         <v>1</v>
       </c>
       <c r="Y11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z11">
         <v>0</v>
       </c>
       <c r="AA11">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB11">
-        <v>-1</v>
-      </c>
-      <c r="AC11">
         <v>1</v>
       </c>
     </row>

</xml_diff>